<commit_message>
Solved Longest Palindromic Subsequence
</commit_message>
<xml_diff>
--- a/DOCS/Leetcode_FULL.xlsx
+++ b/DOCS/Leetcode_FULL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EEA79AC-693C-4165-B77A-2300AC6B2066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D016E948-12CA-485E-BD7A-AA8CADB63D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10770,8 +10770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="D108" sqref="D108"/>
+    <sheetView tabSelected="1" topLeftCell="A478" workbookViewId="0">
+      <selection activeCell="D492" sqref="D492"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -13533,8 +13533,11 @@
       <c r="C194" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E194" s="8" t="s">
-        <v>8</v>
+      <c r="D194" t="s">
+        <v>3367</v>
+      </c>
+      <c r="E194" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="195" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -17684,8 +17687,11 @@
       <c r="C489" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E489" s="8" t="s">
-        <v>8</v>
+      <c r="D489" t="s">
+        <v>3367</v>
+      </c>
+      <c r="E489" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="490" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved a Graph question with djistra, explanation in code file
</commit_message>
<xml_diff>
--- a/DOCS/Leetcode_FULL.xlsx
+++ b/DOCS/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A94C07F8-A953-41CD-8ACD-685A03F68ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B99A23-EA96-47C5-8656-126ECC6663C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6645" uniqueCount="3436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6649" uniqueCount="3445">
   <si>
     <t>ID</t>
   </si>
@@ -10214,9 +10214,6 @@
   </si>
   <si>
     <t>Longer Contiguous Segments of Ones than Zeros</t>
-  </si>
-  <si>
-    <t>1870</t>
   </si>
   <si>
     <t>Minimum Speed to Arrive on Time</t>
@@ -10316,9 +10313,6 @@
     <t>Array With Elements Not Equal to Average of Neighbors</t>
   </si>
   <si>
-    <t>1877</t>
-  </si>
-  <si>
     <t>Explanation in Python File</t>
   </si>
   <si>
@@ -10344,6 +10338,39 @@
   </si>
   <si>
     <t>https://youtu.be/1WugaISSWx8</t>
+  </si>
+  <si>
+    <t>Number of Ways to Arrive at Destination</t>
+  </si>
+  <si>
+    <t>Djikstra with some tweakin</t>
+  </si>
+  <si>
+    <t>2006</t>
+  </si>
+  <si>
+    <t>2007</t>
+  </si>
+  <si>
+    <t>2008</t>
+  </si>
+  <si>
+    <t>2009</t>
+  </si>
+  <si>
+    <t>2010</t>
+  </si>
+  <si>
+    <t>2011</t>
+  </si>
+  <si>
+    <t>2012</t>
+  </si>
+  <si>
+    <t>2013</t>
+  </si>
+  <si>
+    <t>2014</t>
   </si>
 </sst>
 </file>
@@ -10773,8 +10800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A478" workbookViewId="0">
-      <selection activeCell="H496" sqref="H496"/>
+    <sheetView tabSelected="1" topLeftCell="A1680" workbookViewId="0">
+      <selection activeCell="B1702" sqref="B1702"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -10869,7 +10896,7 @@
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>3430</v>
+        <v>3428</v>
       </c>
       <c r="E6" s="9" t="b">
         <v>1</v>
@@ -11710,7 +11737,7 @@
         <v>11</v>
       </c>
       <c r="D65" t="s">
-        <v>3417</v>
+        <v>3416</v>
       </c>
       <c r="E65" s="9" t="b">
         <v>1</v>
@@ -12217,7 +12244,7 @@
         <v>14</v>
       </c>
       <c r="D101" t="s">
-        <v>3403</v>
+        <v>3402</v>
       </c>
       <c r="E101" s="9" t="b">
         <v>1</v>
@@ -12234,7 +12261,7 @@
         <v>14</v>
       </c>
       <c r="D102" t="s">
-        <v>3403</v>
+        <v>3402</v>
       </c>
       <c r="E102" s="9" t="b">
         <v>1</v>
@@ -12265,7 +12292,7 @@
         <v>11</v>
       </c>
       <c r="D104" t="s">
-        <v>3434</v>
+        <v>3432</v>
       </c>
       <c r="E104" s="9" t="b">
         <v>1</v>
@@ -12565,7 +12592,7 @@
         <v>7</v>
       </c>
       <c r="D125" t="s">
-        <v>3428</v>
+        <v>3426</v>
       </c>
       <c r="E125" s="9" t="b">
         <v>1</v>
@@ -13568,7 +13595,7 @@
         <v>11</v>
       </c>
       <c r="D196" t="s">
-        <v>3422</v>
+        <v>3421</v>
       </c>
       <c r="E196" s="9" t="b">
         <v>1</v>
@@ -13613,7 +13640,7 @@
         <v>7</v>
       </c>
       <c r="D199" t="s">
-        <v>3416</v>
+        <v>3415</v>
       </c>
       <c r="E199" s="9" t="b">
         <v>1</v>
@@ -14946,7 +14973,7 @@
         <v>11</v>
       </c>
       <c r="D294" t="s">
-        <v>3420</v>
+        <v>3419</v>
       </c>
       <c r="E294" s="9" t="b">
         <v>1</v>
@@ -15327,7 +15354,7 @@
         <v>11</v>
       </c>
       <c r="D321" t="s">
-        <v>3431</v>
+        <v>3429</v>
       </c>
       <c r="E321" s="9" t="b">
         <v>1</v>
@@ -16618,7 +16645,7 @@
         <v>11</v>
       </c>
       <c r="D413" t="s">
-        <v>3409</v>
+        <v>3408</v>
       </c>
       <c r="E413" s="9" t="b">
         <v>1</v>
@@ -16859,7 +16886,7 @@
         <v>11</v>
       </c>
       <c r="D430" t="s">
-        <v>3406</v>
+        <v>3405</v>
       </c>
       <c r="E430" s="9" t="b">
         <v>1</v>
@@ -17646,7 +17673,7 @@
         <v>11</v>
       </c>
       <c r="D486" t="s">
-        <v>3407</v>
+        <v>3406</v>
       </c>
       <c r="E486" s="9" t="b">
         <v>1</v>
@@ -17806,7 +17833,7 @@
         <v>11</v>
       </c>
       <c r="D497" s="1" t="s">
-        <v>3435</v>
+        <v>3433</v>
       </c>
       <c r="E497" s="9" t="b">
         <v>1</v>
@@ -18663,7 +18690,7 @@
         <v>11</v>
       </c>
       <c r="D558" t="s">
-        <v>3408</v>
+        <v>3407</v>
       </c>
       <c r="E558" s="9" t="b">
         <v>1</v>
@@ -19016,7 +19043,7 @@
         <v>11</v>
       </c>
       <c r="D583" s="1" t="s">
-        <v>3429</v>
+        <v>3427</v>
       </c>
       <c r="E583" s="9" t="b">
         <v>1</v>
@@ -19173,7 +19200,7 @@
         <v>11</v>
       </c>
       <c r="D594" s="1" t="s">
-        <v>3402</v>
+        <v>3401</v>
       </c>
       <c r="E594" s="9" t="b">
         <v>1</v>
@@ -19543,7 +19570,7 @@
         <v>11</v>
       </c>
       <c r="D620" t="s">
-        <v>3433</v>
+        <v>3431</v>
       </c>
       <c r="E620" s="9" t="b">
         <v>1</v>
@@ -20176,7 +20203,7 @@
         <v>11</v>
       </c>
       <c r="D665" t="s">
-        <v>3413</v>
+        <v>3412</v>
       </c>
       <c r="E665" s="9" t="b">
         <v>1</v>
@@ -21467,7 +21494,7 @@
         <v>11</v>
       </c>
       <c r="D757" t="s">
-        <v>3405</v>
+        <v>3404</v>
       </c>
       <c r="E757" s="9" t="b">
         <v>1</v>
@@ -24800,7 +24827,7 @@
         <v>11</v>
       </c>
       <c r="D994" t="s">
-        <v>3404</v>
+        <v>3403</v>
       </c>
       <c r="E994" s="9" t="b">
         <v>1</v>
@@ -24957,7 +24984,7 @@
         <v>11</v>
       </c>
       <c r="D1005" t="s">
-        <v>3405</v>
+        <v>3404</v>
       </c>
       <c r="E1005" s="9" t="b">
         <v>1</v>
@@ -25002,7 +25029,7 @@
         <v>11</v>
       </c>
       <c r="D1008" t="s">
-        <v>3405</v>
+        <v>3404</v>
       </c>
       <c r="E1008" s="9" t="b">
         <v>1</v>
@@ -27175,7 +27202,7 @@
         <v>7</v>
       </c>
       <c r="D1163" t="s">
-        <v>3421</v>
+        <v>3420</v>
       </c>
       <c r="E1163" s="9" t="b">
         <v>1</v>
@@ -27234,7 +27261,7 @@
         <v>7</v>
       </c>
       <c r="D1167" t="s">
-        <v>3419</v>
+        <v>3418</v>
       </c>
       <c r="E1167" s="9" t="b">
         <v>1</v>
@@ -27447,7 +27474,7 @@
         <v>7</v>
       </c>
       <c r="D1182" t="s">
-        <v>3405</v>
+        <v>3404</v>
       </c>
       <c r="E1182" s="9" t="b">
         <v>1</v>
@@ -27590,7 +27617,7 @@
         <v>7</v>
       </c>
       <c r="D1192" t="s">
-        <v>3410</v>
+        <v>3409</v>
       </c>
       <c r="E1192" s="9" t="b">
         <v>1</v>
@@ -28237,7 +28264,7 @@
         <v>11</v>
       </c>
       <c r="D1238" t="s">
-        <v>3418</v>
+        <v>3417</v>
       </c>
       <c r="E1238" s="9" t="b">
         <v>1</v>
@@ -29150,7 +29177,7 @@
         <v>7</v>
       </c>
       <c r="D1303" t="s">
-        <v>3415</v>
+        <v>3414</v>
       </c>
       <c r="E1303" s="9" t="b">
         <v>1</v>
@@ -30475,7 +30502,7 @@
         <v>11</v>
       </c>
       <c r="D1397" t="s">
-        <v>3428</v>
+        <v>3426</v>
       </c>
       <c r="E1397" s="9" t="b">
         <v>1</v>
@@ -30786,7 +30813,7 @@
         <v>11</v>
       </c>
       <c r="D1419" t="s">
-        <v>3432</v>
+        <v>3430</v>
       </c>
       <c r="E1419" s="9" t="b">
         <v>1</v>
@@ -33393,7 +33420,7 @@
         <v>11</v>
       </c>
       <c r="D1605" s="1" t="s">
-        <v>3414</v>
+        <v>3413</v>
       </c>
       <c r="E1605" s="9" t="b">
         <v>1</v>
@@ -34604,8 +34631,8 @@
       </c>
     </row>
     <row r="1692" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1692" s="11">
-        <v>1869</v>
+      <c r="A1692" s="10" t="s">
+        <v>3436</v>
       </c>
       <c r="B1692" s="1" t="s">
         <v>3396</v>
@@ -34618,53 +34645,53 @@
       </c>
     </row>
     <row r="1693" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1693" s="11" t="s">
+      <c r="A1693" s="10" t="s">
+        <v>3437</v>
+      </c>
+      <c r="B1693" s="1" t="s">
         <v>3397</v>
       </c>
-      <c r="B1693" s="1" t="s">
+      <c r="C1693" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1693" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1694" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1694" s="10" t="s">
+        <v>3438</v>
+      </c>
+      <c r="B1694" s="1" t="s">
         <v>3398</v>
       </c>
-      <c r="C1693" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1693" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1694" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1694" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="B1694" s="1" t="s">
+      <c r="C1694" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1694" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1695" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1695" s="10" t="s">
+        <v>3439</v>
+      </c>
+      <c r="B1695" s="1" t="s">
         <v>3399</v>
       </c>
-      <c r="C1694" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1694" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1695" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1695" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="B1695" s="1" t="s">
+      <c r="C1695" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1695" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1696" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1696" s="10" t="s">
+        <v>3440</v>
+      </c>
+      <c r="B1696" s="1" t="s">
         <v>3400</v>
-      </c>
-      <c r="C1695" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1695" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1696" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1696" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="B1696" s="1" t="s">
-        <v>3401</v>
       </c>
       <c r="C1696" s="6" t="s">
         <v>14</v>
@@ -34674,59 +34701,71 @@
       </c>
     </row>
     <row r="1697" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1697" s="11" t="s">
-        <v>184</v>
+      <c r="A1697" s="10" t="s">
+        <v>3441</v>
       </c>
       <c r="B1697" s="1" t="s">
+        <v>3410</v>
+      </c>
+      <c r="C1697" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1697" t="s">
         <v>3411</v>
-      </c>
-      <c r="C1697" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1697" t="s">
-        <v>3412</v>
       </c>
       <c r="E1697" s="9" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="1698" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1698" s="11" t="s">
-        <v>182</v>
+      <c r="A1698" s="10" t="s">
+        <v>3442</v>
       </c>
       <c r="B1698" s="1" t="s">
+        <v>3424</v>
+      </c>
+      <c r="C1698" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1698" t="s">
         <v>3425</v>
-      </c>
-      <c r="C1698" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1698" t="s">
-        <v>3427</v>
       </c>
       <c r="E1698" s="9" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="1699" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1699" s="11" t="s">
-        <v>180</v>
+      <c r="A1699" s="10" t="s">
+        <v>3443</v>
       </c>
       <c r="B1699" s="1" t="s">
+        <v>3422</v>
+      </c>
+      <c r="C1699" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1699" t="s">
         <v>3423</v>
-      </c>
-      <c r="C1699" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1699" t="s">
-        <v>3424</v>
       </c>
       <c r="E1699" s="9" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="1700" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1700" s="11" t="s">
-        <v>3426</v>
+      <c r="A1700" s="10" t="s">
+        <v>3444</v>
+      </c>
+      <c r="B1700" s="1" t="s">
+        <v>3434</v>
+      </c>
+      <c r="C1700" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1700" t="s">
+        <v>3435</v>
+      </c>
+      <c r="E1700" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -36441,8 +36480,9 @@
     <hyperlink ref="D1605" r:id="rId1703" xr:uid="{0D40AF47-4380-4A3C-B92C-6961B6E391DF}"/>
     <hyperlink ref="D583" r:id="rId1704" xr:uid="{61FA88FA-2D4F-4048-BCC5-501F7B008612}"/>
     <hyperlink ref="D497" r:id="rId1705" xr:uid="{9150FFFD-9A4C-4ADB-B5C1-47FF5C6FB818}"/>
+    <hyperlink ref="B1700" r:id="rId1706" xr:uid="{91F20E79-BADE-4AF0-B4AA-A67651693AA5}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1706"/>
+  <pageSetup orientation="portrait" r:id="rId1707"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Solved a problem with DSU
</commit_message>
<xml_diff>
--- a/DOCS/Leetcode_FULL.xlsx
+++ b/DOCS/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B99A23-EA96-47C5-8656-126ECC6663C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F927AA-E898-4495-8ADD-921C5D05DCB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6649" uniqueCount="3445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6649" uniqueCount="3446">
   <si>
     <t>ID</t>
   </si>
@@ -10371,6 +10371,9 @@
   </si>
   <si>
     <t>2014</t>
+  </si>
+  <si>
+    <t>DSU</t>
   </si>
 </sst>
 </file>
@@ -10800,8 +10803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1680" workbookViewId="0">
-      <selection activeCell="B1702" sqref="B1702"/>
+    <sheetView tabSelected="1" topLeftCell="A523" workbookViewId="0">
+      <selection activeCell="I533" sqref="I533"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -18353,8 +18356,11 @@
       <c r="C534" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E534" s="8" t="s">
-        <v>8</v>
+      <c r="D534" t="s">
+        <v>3445</v>
+      </c>
+      <c r="E534" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="535" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved a Maximum cost path in graph path type problem using Djikstra
</commit_message>
<xml_diff>
--- a/DOCS/Leetcode_FULL.xlsx
+++ b/DOCS/Leetcode_FULL.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\DOCS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TIME BOMB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F927AA-E898-4495-8ADD-921C5D05DCB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB98AF16-1164-4D0C-91AD-631E943F0EE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6649" uniqueCount="3446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6649" uniqueCount="3447">
   <si>
     <t>ID</t>
   </si>
@@ -10374,6 +10374,9 @@
   </si>
   <si>
     <t>DSU</t>
+  </si>
+  <si>
+    <t>Solved Using Dijkstra</t>
   </si>
 </sst>
 </file>
@@ -10803,8 +10806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A523" workbookViewId="0">
-      <selection activeCell="I533" sqref="I533"/>
+    <sheetView tabSelected="1" topLeftCell="A1167" workbookViewId="0">
+      <selection activeCell="D1171" sqref="D1171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -27423,8 +27426,11 @@
       <c r="C1178" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1178" s="8" t="s">
-        <v>8</v>
+      <c r="D1178" t="s">
+        <v>3446</v>
+      </c>
+      <c r="E1178" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1179" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Unique Paths II---- DP
</commit_message>
<xml_diff>
--- a/DOCS/Leetcode_FULL.xlsx
+++ b/DOCS/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{563149F0-AB4C-4E6C-BE87-CAEF6E888AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F1AF4D-E3B6-4553-BFB0-F5E8EEADDBB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10809,8 +10809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A318" workbookViewId="0">
-      <selection activeCell="D332" sqref="D332"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -11731,8 +11731,11 @@
       <c r="C64" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E64" s="8" t="s">
-        <v>8</v>
+      <c r="D64" t="s">
+        <v>3416</v>
+      </c>
+      <c r="E64" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Inversion Count related problem
</commit_message>
<xml_diff>
--- a/DOCS/Leetcode_FULL.xlsx
+++ b/DOCS/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F68CB4-DE3D-4837-BD21-B375D6A5698E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3051FAD-A16A-424A-B49B-66A0A9CE2BC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6649" uniqueCount="3448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6649" uniqueCount="3449">
   <si>
     <t>ID</t>
   </si>
@@ -10380,6 +10380,9 @@
   </si>
   <si>
     <t>Bucket Sort, Refer any youtube video</t>
+  </si>
+  <si>
+    <t>Inversion Count</t>
   </si>
 </sst>
 </file>
@@ -10809,8 +10812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="D155" sqref="D155"/>
+    <sheetView tabSelected="1" topLeftCell="A704" workbookViewId="0">
+      <selection activeCell="D716" sqref="D716"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -20926,8 +20929,11 @@
       <c r="C715" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E715" s="8" t="s">
-        <v>8</v>
+      <c r="D715" t="s">
+        <v>3448</v>
+      </c>
+      <c r="E715" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="716" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
A Graph question solved
</commit_message>
<xml_diff>
--- a/DOCS/Leetcode_FULL.xlsx
+++ b/DOCS/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3051FAD-A16A-424A-B49B-66A0A9CE2BC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415751BA-51E8-49AB-BE12-53532B2FC2FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6649" uniqueCount="3449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6649" uniqueCount="3450">
   <si>
     <t>ID</t>
   </si>
@@ -10383,6 +10383,9 @@
   </si>
   <si>
     <t>Inversion Count</t>
+  </si>
+  <si>
+    <t>DFS</t>
   </si>
 </sst>
 </file>
@@ -10812,8 +10815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A704" workbookViewId="0">
-      <selection activeCell="D716" sqref="D716"/>
+    <sheetView tabSelected="1" topLeftCell="A734" workbookViewId="0">
+      <selection activeCell="D748" sqref="D748"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -21352,8 +21355,11 @@
       <c r="C745" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E745" s="8" t="s">
-        <v>8</v>
+      <c r="D745" t="s">
+        <v>3449</v>
+      </c>
+      <c r="E745" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="746" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Stone Game II
</commit_message>
<xml_diff>
--- a/DOCS/Leetcode_FULL.xlsx
+++ b/DOCS/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A6B1501-F914-41E5-88DD-2FF04A4936F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC5F4F1B-5E33-4335-B22D-1BE98D359906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6648" uniqueCount="3454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6648" uniqueCount="3455">
   <si>
     <t>ID</t>
   </si>
@@ -10398,6 +10398,9 @@
   </si>
   <si>
     <t>DP -&gt; Explanation in File for O(n2) optimization</t>
+  </si>
+  <si>
+    <t>Game Theory DP</t>
   </si>
 </sst>
 </file>
@@ -10827,8 +10830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="F132" sqref="F132"/>
+    <sheetView tabSelected="1" topLeftCell="A1110" workbookViewId="0">
+      <selection activeCell="D1121" sqref="D1121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -26673,8 +26676,11 @@
       <c r="C1121" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1121" s="8" t="s">
-        <v>8</v>
+      <c r="D1121" t="s">
+        <v>3454</v>
+      </c>
+      <c r="E1121" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1122" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Stone Game VII
</commit_message>
<xml_diff>
--- a/DOCS/Leetcode_FULL.xlsx
+++ b/DOCS/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC5F4F1B-5E33-4335-B22D-1BE98D359906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13CE0FD9-0E46-45E6-9586-B510B030FC69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10830,8 +10830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1110" workbookViewId="0">
-      <selection activeCell="D1121" sqref="D1121"/>
+    <sheetView tabSelected="1" topLeftCell="A1534" workbookViewId="0">
+      <selection activeCell="E1545" sqref="E1545"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -32651,8 +32651,11 @@
       <c r="C1545" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1545" s="8" t="s">
-        <v>8</v>
+      <c r="D1545" t="s">
+        <v>3454</v>
+      </c>
+      <c r="E1545" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1546" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Convert BST to Greater tree
</commit_message>
<xml_diff>
--- a/DOCS/Leetcode_FULL.xlsx
+++ b/DOCS/Leetcode_FULL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0468732E-EFA1-46BA-B790-33F7FA0DB8AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{175BA918-0C6C-49EE-BFBA-CA3E3454150E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6647" uniqueCount="3457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6646" uniqueCount="3457">
   <si>
     <t>ID</t>
   </si>
@@ -10836,8 +10836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A571" workbookViewId="0">
-      <selection activeCell="D582" sqref="D582"/>
+    <sheetView tabSelected="1" topLeftCell="A496" workbookViewId="0">
+      <selection activeCell="D509" sqref="D509"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -18063,8 +18063,8 @@
       <c r="C509" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E509" s="8" t="s">
-        <v>8</v>
+      <c r="E509" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="510" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Complete Binary Tree Inserter
</commit_message>
<xml_diff>
--- a/DOCS/Leetcode_FULL.xlsx
+++ b/DOCS/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{175BA918-0C6C-49EE-BFBA-CA3E3454150E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677243A3-383A-47CB-A581-7C088D0447D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10836,8 +10836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A496" workbookViewId="0">
-      <selection activeCell="D509" sqref="D509"/>
+    <sheetView tabSelected="1" topLeftCell="A860" workbookViewId="0">
+      <selection activeCell="D874" sqref="D874"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -23195,8 +23195,11 @@
       <c r="C873" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E873" s="8" t="s">
-        <v>8</v>
+      <c r="D873" t="s">
+        <v>3404</v>
+      </c>
+      <c r="E873" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="874" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Construct K Palindrome Strings
</commit_message>
<xml_diff>
--- a/DOCS/Leetcode_FULL.xlsx
+++ b/DOCS/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677243A3-383A-47CB-A581-7C088D0447D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F36116-5AE6-4CCD-9B65-145D66B1B626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6646" uniqueCount="3457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6645" uniqueCount="3457">
   <si>
     <t>ID</t>
   </si>
@@ -10836,8 +10836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A860" workbookViewId="0">
-      <selection activeCell="D874" sqref="D874"/>
+    <sheetView tabSelected="1" topLeftCell="A1286" workbookViewId="0">
+      <selection activeCell="E1299" sqref="E1299"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -29207,8 +29207,8 @@
       <c r="C1299" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1299" s="8" t="s">
-        <v>8</v>
+      <c r="E1299" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1300" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Word Ladder and Binary Tree Level Order Traversal
</commit_message>
<xml_diff>
--- a/DOCS/Leetcode_FULL.xlsx
+++ b/DOCS/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6AA9499-482E-4AFC-964C-EE4B02137266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA011B62-CA44-4ADC-A892-7F29FFFBEB6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6645" uniqueCount="3459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6645" uniqueCount="3460">
   <si>
     <t>ID</t>
   </si>
@@ -10413,6 +10413,9 @@
   </si>
   <si>
     <t>FInding Tree Center(s)</t>
+  </si>
+  <si>
+    <t>BFS, Explanation in code file</t>
   </si>
 </sst>
 </file>
@@ -10842,8 +10845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="E148" sqref="E148"/>
+    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
+      <selection activeCell="D128" sqref="D128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -12687,8 +12690,11 @@
       <c r="C128" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E128" s="8" t="s">
-        <v>8</v>
+      <c r="D128" t="s">
+        <v>3459</v>
+      </c>
+      <c r="E128" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved First Problem using Digit Sum
</commit_message>
<xml_diff>
--- a/DOCS/Leetcode_FULL.xlsx
+++ b/DOCS/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA011B62-CA44-4ADC-A892-7F29FFFBEB6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C598B5D-2B0B-40B0-A5A0-847DADAC8FC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6645" uniqueCount="3460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6645" uniqueCount="3461">
   <si>
     <t>ID</t>
   </si>
@@ -10416,6 +10416,9 @@
   </si>
   <si>
     <t>BFS, Explanation in code file</t>
+  </si>
+  <si>
+    <t>Digit DP + Math. Check OneNote too and explanation in file</t>
   </si>
 </sst>
 </file>
@@ -10845,8 +10848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="D128" sqref="D128"/>
+    <sheetView tabSelected="1" topLeftCell="A843" workbookViewId="0">
+      <selection activeCell="D857" sqref="D857"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -22978,8 +22981,11 @@
       <c r="C856" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E856" s="8" t="s">
-        <v>8</v>
+      <c r="D856" t="s">
+        <v>3460</v>
+      </c>
+      <c r="E856" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="857" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved 3 problems leetcode
</commit_message>
<xml_diff>
--- a/DOCS/Leetcode_FULL.xlsx
+++ b/DOCS/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C598B5D-2B0B-40B0-A5A0-847DADAC8FC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D870B64F-7DD5-4422-BF15-371D31876529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6645" uniqueCount="3461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6645" uniqueCount="3463">
   <si>
     <t>ID</t>
   </si>
@@ -10419,6 +10419,12 @@
   </si>
   <si>
     <t>Digit DP + Math. Check OneNote too and explanation in file</t>
+  </si>
+  <si>
+    <t>Similar to Word Ladder, with some logic changes</t>
+  </si>
+  <si>
+    <t>Explanation Here</t>
   </si>
 </sst>
 </file>
@@ -10848,8 +10854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A843" workbookViewId="0">
-      <selection activeCell="D857" sqref="D857"/>
+    <sheetView tabSelected="1" topLeftCell="A1301" workbookViewId="0">
+      <selection activeCell="E1314" sqref="E1314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -12679,8 +12685,11 @@
       <c r="C127" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E127" s="8" t="s">
-        <v>8</v>
+      <c r="D127" t="s">
+        <v>3461</v>
+      </c>
+      <c r="E127" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -16235,8 +16244,11 @@
       <c r="C378" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E378" s="8" t="s">
-        <v>8</v>
+      <c r="D378" s="1" t="s">
+        <v>3462</v>
+      </c>
+      <c r="E378" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="379" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -29447,8 +29459,11 @@
       <c r="C1314" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E1314" s="8" t="s">
-        <v>8</v>
+      <c r="D1314" t="s">
+        <v>3454</v>
+      </c>
+      <c r="E1314" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1315" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -36599,8 +36614,9 @@
     <hyperlink ref="D497" r:id="rId1705" xr:uid="{9150FFFD-9A4C-4ADB-B5C1-47FF5C6FB818}"/>
     <hyperlink ref="B1700" r:id="rId1706" xr:uid="{91F20E79-BADE-4AF0-B4AA-A67651693AA5}"/>
     <hyperlink ref="D206" r:id="rId1707" xr:uid="{EC68EA4A-1B48-4B31-9A2F-54416F0AF1B4}"/>
+    <hyperlink ref="D378" r:id="rId1708" xr:uid="{F9608593-C7AC-43AE-96E3-16072155D06D}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1708"/>
+  <pageSetup orientation="portrait" r:id="rId1709"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Solved Maximum XOR of Two Numbers in an Array
</commit_message>
<xml_diff>
--- a/DOCS/Leetcode_FULL.xlsx
+++ b/DOCS/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D870B64F-7DD5-4422-BF15-371D31876529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78E31B7-F451-4BC1-8913-49A1FF8DAFB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6645" uniqueCount="3463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6645" uniqueCount="3465">
   <si>
     <t>ID</t>
   </si>
@@ -10425,6 +10425,12 @@
   </si>
   <si>
     <t>Explanation Here</t>
+  </si>
+  <si>
+    <t>Bit Trie for finding Max Xor. Explanation given.</t>
+  </si>
+  <si>
+    <t>Bit Trie for MAX Xor</t>
   </si>
 </sst>
 </file>
@@ -10854,8 +10860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1301" workbookViewId="0">
-      <selection activeCell="E1314" sqref="E1314"/>
+    <sheetView tabSelected="1" topLeftCell="A392" workbookViewId="0">
+      <selection activeCell="E405" sqref="E405"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -16625,8 +16631,11 @@
       <c r="C405" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E405" s="8" t="s">
-        <v>8</v>
+      <c r="D405" t="s">
+        <v>3464</v>
+      </c>
+      <c r="E405" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="406" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -32935,8 +32944,11 @@
       <c r="C1561" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E1561" s="8" t="s">
-        <v>8</v>
+      <c r="D1561" t="s">
+        <v>3463</v>
+      </c>
+      <c r="E1561" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1562" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Merge In Between Linked Lists
</commit_message>
<xml_diff>
--- a/DOCS/Leetcode_FULL.xlsx
+++ b/DOCS/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78E31B7-F451-4BC1-8913-49A1FF8DAFB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D47C7366-7F4D-454F-B486-C3A5B7F8DBB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6645" uniqueCount="3465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6644" uniqueCount="3465">
   <si>
     <t>ID</t>
   </si>
@@ -10860,8 +10860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A392" workbookViewId="0">
-      <selection activeCell="E405" sqref="E405"/>
+    <sheetView tabSelected="1" topLeftCell="A1494" workbookViewId="0">
+      <selection activeCell="E1507" sqref="E1507"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -32185,8 +32185,8 @@
       <c r="C1507" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1507" s="8" t="s">
-        <v>8</v>
+      <c r="E1507" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1508" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved a hard problem of seive and DSU
</commit_message>
<xml_diff>
--- a/DOCS/Leetcode_FULL.xlsx
+++ b/DOCS/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8B3D79-F2D4-4050-918A-FC49639C4C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A2B30B0-5007-45FA-9BEE-D8633ABA4853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6644" uniqueCount="3468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6644" uniqueCount="3469">
   <si>
     <t>ID</t>
   </si>
@@ -10440,6 +10440,9 @@
   </si>
   <si>
     <t>https://youtu.be/0do2734xhnU</t>
+  </si>
+  <si>
+    <t>DSU + Sieve of Eratothenes</t>
   </si>
 </sst>
 </file>
@@ -10869,8 +10872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A516" workbookViewId="0">
-      <selection activeCell="D530" sqref="D530"/>
+    <sheetView tabSelected="1" topLeftCell="A1098" workbookViewId="0">
+      <selection activeCell="E1108" sqref="E1108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -26578,8 +26581,11 @@
       <c r="C1108" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E1108" s="8" t="s">
-        <v>8</v>
+      <c r="D1108" t="s">
+        <v>3468</v>
+      </c>
+      <c r="E1108" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1109" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Network Time Delay
</commit_message>
<xml_diff>
--- a/DOCS/Leetcode_FULL.xlsx
+++ b/DOCS/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEBBFB67-C70A-4D6D-A206-63334E06E8C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50B56ED-2950-4BD3-AA49-73669772B703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6645" uniqueCount="3471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6645" uniqueCount="3472">
   <si>
     <t>ID</t>
   </si>
@@ -10449,6 +10449,9 @@
   </si>
   <si>
     <t>Divide and Conquer or LR DP</t>
+  </si>
+  <si>
+    <t>Dijkstra and then send largest distance</t>
   </si>
 </sst>
 </file>
@@ -10878,8 +10881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A283" workbookViewId="0">
-      <selection activeCell="D296" sqref="D296"/>
+    <sheetView tabSelected="1" topLeftCell="A656" workbookViewId="0">
+      <selection activeCell="D669" sqref="D669"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -20399,8 +20402,11 @@
       <c r="C669" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E669" s="8" t="s">
-        <v>8</v>
+      <c r="D669" t="s">
+        <v>3471</v>
+      </c>
+      <c r="E669" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="670" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Longest Substring with At Least K Repeating Characters
</commit_message>
<xml_diff>
--- a/DOCS/Leetcode_FULL.xlsx
+++ b/DOCS/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50B56ED-2950-4BD3-AA49-73669772B703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A429952C-95BE-4B7C-B5C4-2E62056E707C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10881,8 +10881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A656" workbookViewId="0">
-      <selection activeCell="D669" sqref="D669"/>
+    <sheetView tabSelected="1" topLeftCell="A366" workbookViewId="0">
+      <selection activeCell="D379" sqref="D379"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -16294,8 +16294,11 @@
       <c r="C379" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E379" s="8" t="s">
-        <v>8</v>
+      <c r="D379" t="s">
+        <v>3426</v>
+      </c>
+      <c r="E379" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="380" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Longest Increasing Path in a Matrix
</commit_message>
<xml_diff>
--- a/DOCS/Leetcode_FULL.xlsx
+++ b/DOCS/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A429952C-95BE-4B7C-B5C4-2E62056E707C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4771E9E3-89A9-45B8-91F7-67BC2B04E041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6645" uniqueCount="3472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6645" uniqueCount="3473">
   <si>
     <t>ID</t>
   </si>
@@ -10452,6 +10452,9 @@
   </si>
   <si>
     <t>Dijkstra and then send largest distance</t>
+  </si>
+  <si>
+    <t>DP + DFS: Explanation in One Note</t>
   </si>
 </sst>
 </file>
@@ -10881,8 +10884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A366" workbookViewId="0">
-      <selection activeCell="D379" sqref="D379"/>
+    <sheetView tabSelected="1" topLeftCell="A300" workbookViewId="0">
+      <selection activeCell="D317" sqref="D317"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -15361,8 +15364,11 @@
       <c r="C313" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E313" s="8" t="s">
-        <v>8</v>
+      <c r="D313" t="s">
+        <v>3472</v>
+      </c>
+      <c r="E313" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="314" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Max Increase to Keep City SKyline
</commit_message>
<xml_diff>
--- a/DOCS/Leetcode_FULL.xlsx
+++ b/DOCS/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4771E9E3-89A9-45B8-91F7-67BC2B04E041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D875FB6-20AD-4ED0-8435-D9F3FA26C658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10884,8 +10884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A300" workbookViewId="0">
-      <selection activeCell="D317" sqref="D317"/>
+    <sheetView tabSelected="1" topLeftCell="A737" workbookViewId="0">
+      <selection activeCell="E750" sqref="E750"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -21557,8 +21557,11 @@
       <c r="C750" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E750" s="8" t="s">
-        <v>8</v>
+      <c r="D750" t="s">
+        <v>3404</v>
+      </c>
+      <c r="E750" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="751" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved 2 problems leetcode
</commit_message>
<xml_diff>
--- a/DOCS/Leetcode_FULL.xlsx
+++ b/DOCS/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D64E3C-791D-4DFA-A18A-B6D5E825B6AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42BCD1DF-D183-42DD-BADC-E91F1E3B7075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6645" uniqueCount="3474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6648" uniqueCount="3476">
   <si>
     <t>ID</t>
   </si>
@@ -10458,6 +10458,12 @@
   </si>
   <si>
     <t>Partial Sums</t>
+  </si>
+  <si>
+    <t>Maximum Fruits Harvested After at Most K Steps</t>
+  </si>
+  <si>
+    <t>Prefix Sum Tricky</t>
   </si>
 </sst>
 </file>
@@ -10554,7 +10560,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -10581,6 +10587,9 @@
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -10885,10 +10894,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1700"/>
+  <dimension ref="A1:E1701"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1057" workbookViewId="0">
-      <selection activeCell="E1079" sqref="E1079"/>
+    <sheetView tabSelected="1" topLeftCell="A1204" workbookViewId="0">
+      <selection activeCell="D1218" sqref="D1218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -28164,8 +28173,11 @@
       <c r="C1217" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1217" s="8" t="s">
-        <v>8</v>
+      <c r="D1217" t="s">
+        <v>3404</v>
+      </c>
+      <c r="E1217" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1218" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -34975,6 +34987,23 @@
         <v>3435</v>
       </c>
       <c r="E1700" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1701" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1701" s="12">
+        <v>2015</v>
+      </c>
+      <c r="B1701" s="1" t="s">
+        <v>3474</v>
+      </c>
+      <c r="C1701" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1701" t="s">
+        <v>3475</v>
+      </c>
+      <c r="E1701" s="9" t="b">
         <v>1</v>
       </c>
     </row>
@@ -36695,8 +36724,9 @@
     <hyperlink ref="D378" r:id="rId1708" xr:uid="{F9608593-C7AC-43AE-96E3-16072155D06D}"/>
     <hyperlink ref="D709" r:id="rId1709" xr:uid="{CB86AB24-6B0E-45B1-BC77-000B12DAA422}"/>
     <hyperlink ref="D85" r:id="rId1710" xr:uid="{5EC41503-5BF9-4FF5-8D36-A157E1B8AAC6}"/>
+    <hyperlink ref="B1701" r:id="rId1711" xr:uid="{A58925E6-DAF0-4F95-A761-4E0C09A5E431}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1711"/>
+  <pageSetup orientation="portrait" r:id="rId1712"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Solved a couple of questions
</commit_message>
<xml_diff>
--- a/DOCS/Leetcode_FULL.xlsx
+++ b/DOCS/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE92B56B-5AB5-469C-AEB0-27367A17E65B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D0A8CF-9FA0-4448-8A58-B450C12ED6A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6648" uniqueCount="3480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6647" uniqueCount="3481">
   <si>
     <t>ID</t>
   </si>
@@ -10476,6 +10476,9 @@
   </si>
   <si>
     <t>Monoqueue</t>
+  </si>
+  <si>
+    <t>Monoque, See vid link, tricky</t>
   </si>
 </sst>
 </file>
@@ -10908,8 +10911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1701"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A211" workbookViewId="0">
-      <selection activeCell="D224" sqref="D224"/>
+    <sheetView tabSelected="1" topLeftCell="A1483" workbookViewId="0">
+      <selection activeCell="E1484" sqref="E1484"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -30573,8 +30576,11 @@
       <c r="C1385" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E1385" s="8" t="s">
-        <v>8</v>
+      <c r="D1385" t="s">
+        <v>3480</v>
+      </c>
+      <c r="E1385" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1386" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -31965,8 +31971,8 @@
       <c r="C1484" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1484" s="8" t="s">
-        <v>8</v>
+      <c r="E1484" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1485" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved All palindrome Paritioning questions
</commit_message>
<xml_diff>
--- a/DOCS/Leetcode_FULL.xlsx
+++ b/DOCS/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6609D6-3142-49FC-BCB3-032330A710D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39010DE-E5C2-459D-8AC9-52F4C8FCFC47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10920,8 +10920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1701"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1210" workbookViewId="0">
-      <selection activeCell="D1223" sqref="D1223"/>
+    <sheetView tabSelected="1" topLeftCell="A1579" workbookViewId="0">
+      <selection activeCell="D1593" sqref="D1593"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -33510,8 +33510,11 @@
       <c r="C1592" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E1592" s="8" t="s">
-        <v>8</v>
+      <c r="D1592" t="s">
+        <v>3412</v>
+      </c>
+      <c r="E1592" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1593" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved upti Stone Game V
</commit_message>
<xml_diff>
--- a/DOCS/Leetcode_FULL.xlsx
+++ b/DOCS/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFEC00C1-16A3-40F1-B491-3B1AE7C300D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5132C7-199B-4567-8922-02882BF350CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10920,8 +10920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1701"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1367" workbookViewId="0">
-      <selection activeCell="D1381" sqref="D1381"/>
+    <sheetView tabSelected="1" topLeftCell="A1426" workbookViewId="0">
+      <selection activeCell="D1440" sqref="D1440"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -31362,8 +31362,11 @@
       <c r="C1439" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E1439" s="8" t="s">
-        <v>8</v>
+      <c r="D1439" t="s">
+        <v>3454</v>
+      </c>
+      <c r="E1439" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1440" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved upto Stone Game VI
</commit_message>
<xml_diff>
--- a/DOCS/Leetcode_FULL.xlsx
+++ b/DOCS/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5132C7-199B-4567-8922-02882BF350CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E445B0CD-2172-4824-83D2-D4A9BB665678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6647" uniqueCount="3484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6647" uniqueCount="3485">
   <si>
     <t>ID</t>
   </si>
@@ -10488,6 +10488,9 @@
   </si>
   <si>
     <t>Explanation in OneNote and code File</t>
+  </si>
+  <si>
+    <t>Sort based on largest alice[i]+bob[i]</t>
   </si>
 </sst>
 </file>
@@ -10920,8 +10923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1701"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1426" workbookViewId="0">
-      <selection activeCell="D1440" sqref="D1440"/>
+    <sheetView tabSelected="1" topLeftCell="A1514" workbookViewId="0">
+      <selection activeCell="D1527" sqref="D1527"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -32597,8 +32600,11 @@
       <c r="C1527" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1527" s="8" t="s">
-        <v>8</v>
+      <c r="D1527" t="s">
+        <v>3484</v>
+      </c>
+      <c r="E1527" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1528" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Maximum Level Sum of a Bianry Tree
</commit_message>
<xml_diff>
--- a/DOCS/Leetcode_FULL.xlsx
+++ b/DOCS/Leetcode_FULL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E445B0CD-2172-4824-83D2-D4A9BB665678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D660D5-6D8A-469C-BE07-BE77A56FFCFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10923,8 +10923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1701"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1514" workbookViewId="0">
-      <selection activeCell="D1527" sqref="D1527"/>
+    <sheetView tabSelected="1" topLeftCell="A1014" workbookViewId="0">
+      <selection activeCell="D1027" sqref="D1027"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -25525,8 +25525,11 @@
       <c r="C1027" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1027" s="8" t="s">
-        <v>8</v>
+      <c r="D1027" t="s">
+        <v>3411</v>
+      </c>
+      <c r="E1027" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1028" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Stone Game VIII
</commit_message>
<xml_diff>
--- a/DOCS/Leetcode_FULL.xlsx
+++ b/DOCS/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D660D5-6D8A-469C-BE07-BE77A56FFCFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382DE74B-4C60-4C00-BDA2-28A8A17727EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6647" uniqueCount="3485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6647" uniqueCount="3486">
   <si>
     <t>ID</t>
   </si>
@@ -10491,6 +10491,9 @@
   </si>
   <si>
     <t>Sort based on largest alice[i]+bob[i]</t>
+  </si>
+  <si>
+    <t>Tricky DP optimization</t>
   </si>
 </sst>
 </file>
@@ -10923,8 +10926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1701"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1014" workbookViewId="0">
-      <selection activeCell="D1027" sqref="D1027"/>
+    <sheetView tabSelected="1" topLeftCell="A1682" workbookViewId="0">
+      <selection activeCell="D1695" sqref="D1695"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -34976,8 +34979,11 @@
       <c r="C1695" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E1695" s="8" t="s">
-        <v>8</v>
+      <c r="D1695" t="s">
+        <v>3485</v>
+      </c>
+      <c r="E1695" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1696" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved Sum of Subarray Ranges
</commit_message>
<xml_diff>
--- a/DOCS/Leetcode_FULL.xlsx
+++ b/DOCS/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382DE74B-4C60-4C00-BDA2-28A8A17727EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E34B4AA-3F0E-4001-80DA-96AEFF429FE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6647" uniqueCount="3486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6650" uniqueCount="3489">
   <si>
     <t>ID</t>
   </si>
@@ -10494,6 +10494,15 @@
   </si>
   <si>
     <t>Tricky DP optimization</t>
+  </si>
+  <si>
+    <t>Sum of Subarray Ranges</t>
+  </si>
+  <si>
+    <t>Monotonic Stack's Very Good Use</t>
+  </si>
+  <si>
+    <t>Good use of Monotonic Stack/ Queue</t>
   </si>
 </sst>
 </file>
@@ -10924,10 +10933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1701"/>
+  <dimension ref="A1:E1702"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1682" workbookViewId="0">
-      <selection activeCell="D1695" sqref="D1695"/>
+    <sheetView tabSelected="1" topLeftCell="A848" workbookViewId="0">
+      <selection activeCell="D862" sqref="D862"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -23177,8 +23186,11 @@
       <c r="C861" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E861" s="8" t="s">
-        <v>8</v>
+      <c r="D861" t="s">
+        <v>3488</v>
+      </c>
+      <c r="E861" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="862" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -35082,6 +35094,23 @@
         <v>3475</v>
       </c>
       <c r="E1701" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1702" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1702" s="12">
+        <v>2016</v>
+      </c>
+      <c r="B1702" s="1" t="s">
+        <v>3486</v>
+      </c>
+      <c r="C1702" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1702" t="s">
+        <v>3487</v>
+      </c>
+      <c r="E1702" s="9" t="b">
         <v>1</v>
       </c>
     </row>
@@ -36803,8 +36832,9 @@
     <hyperlink ref="D709" r:id="rId1709" xr:uid="{CB86AB24-6B0E-45B1-BC77-000B12DAA422}"/>
     <hyperlink ref="D85" r:id="rId1710" xr:uid="{5EC41503-5BF9-4FF5-8D36-A157E1B8AAC6}"/>
     <hyperlink ref="B1701" r:id="rId1711" xr:uid="{A58925E6-DAF0-4F95-A761-4E0C09A5E431}"/>
+    <hyperlink ref="B1702" r:id="rId1712" xr:uid="{F81604E5-E7CC-466A-83EC-DB2C3214D809}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1712"/>
+  <pageSetup orientation="portrait" r:id="rId1713"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Solved a few questions
</commit_message>
<xml_diff>
--- a/DOCS/Leetcode_FULL.xlsx
+++ b/DOCS/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DBA82A6-EB6C-4E38-8F2A-673F48545D7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0822AF8B-0E83-47F9-AFFB-83400DF5B510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6650" uniqueCount="3490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6650" uniqueCount="3491">
   <si>
     <t>ID</t>
   </si>
@@ -10506,6 +10506,9 @@
   </si>
   <si>
     <t>Two Pointer</t>
+  </si>
+  <si>
+    <t>Hard and V. IMP DP</t>
   </si>
 </sst>
 </file>
@@ -10938,8 +10941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1702"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A784" workbookViewId="0">
-      <selection activeCell="D797" sqref="D797"/>
+    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
+      <selection activeCell="D175" sqref="D175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -13468,8 +13471,11 @@
       <c r="C175" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E175" s="8" t="s">
-        <v>8</v>
+      <c r="D175" t="s">
+        <v>3490</v>
+      </c>
+      <c r="E175" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="176" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved lot of problems
</commit_message>
<xml_diff>
--- a/DOCS/Leetcode_FULL.xlsx
+++ b/DOCS/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0822AF8B-0E83-47F9-AFFB-83400DF5B510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597BD402-2FB5-4F90-BE46-C068458C9ECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6650" uniqueCount="3491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6649" uniqueCount="3493">
   <si>
     <t>ID</t>
   </si>
@@ -10509,6 +10509,12 @@
   </si>
   <si>
     <t>Hard and V. IMP DP</t>
+  </si>
+  <si>
+    <t>https://youtu.be/j6IHk2cH58I</t>
+  </si>
+  <si>
+    <t>Find factors for num+1 and num+2</t>
   </si>
 </sst>
 </file>
@@ -10941,8 +10947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1702"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
-      <selection activeCell="D175" sqref="D175"/>
+    <sheetView tabSelected="1" topLeftCell="A1135" workbookViewId="0">
+      <selection activeCell="D1148" sqref="D1148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -11123,8 +11129,11 @@
       <c r="C12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>8</v>
+      <c r="D12" t="s">
+        <v>3367</v>
+      </c>
+      <c r="E12" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -13017,8 +13026,8 @@
       <c r="C143" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E143" s="8" t="s">
-        <v>8</v>
+      <c r="E143" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -17064,8 +17073,11 @@
       <c r="C428" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E428" s="8" t="s">
-        <v>8</v>
+      <c r="D428" s="1" t="s">
+        <v>3491</v>
+      </c>
+      <c r="E428" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="429" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -21539,11 +21551,14 @@
       <c r="B744" s="1" t="s">
         <v>1879</v>
       </c>
-      <c r="C744" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E744" s="8" t="s">
-        <v>8</v>
+      <c r="C744" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D744" t="s">
+        <v>3412</v>
+      </c>
+      <c r="E744" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="745" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -27261,8 +27276,11 @@
       <c r="C1148" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1148" s="8" t="s">
-        <v>8</v>
+      <c r="D1148" t="s">
+        <v>3492</v>
+      </c>
+      <c r="E1148" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1149" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -36845,8 +36863,9 @@
     <hyperlink ref="D85" r:id="rId1710" xr:uid="{5EC41503-5BF9-4FF5-8D36-A157E1B8AAC6}"/>
     <hyperlink ref="B1701" r:id="rId1711" xr:uid="{A58925E6-DAF0-4F95-A761-4E0C09A5E431}"/>
     <hyperlink ref="B1702" r:id="rId1712" xr:uid="{F81604E5-E7CC-466A-83EC-DB2C3214D809}"/>
+    <hyperlink ref="D428" r:id="rId1713" xr:uid="{18096D3C-0C4B-45BD-BBFD-FF3BB6761391}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1713"/>
+  <pageSetup orientation="portrait" r:id="rId1714"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Solved 2 Hard problems
</commit_message>
<xml_diff>
--- a/DOCS/Leetcode_FULL.xlsx
+++ b/DOCS/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597BD402-2FB5-4F90-BE46-C068458C9ECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24020AC-B6AF-4494-AF14-0595486C17F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6649" uniqueCount="3493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6649" uniqueCount="3494">
   <si>
     <t>ID</t>
   </si>
@@ -10515,6 +10515,9 @@
   </si>
   <si>
     <t>Find factors for num+1 and num+2</t>
+  </si>
+  <si>
+    <t>DP+ MonoQueue, New Concept</t>
   </si>
 </sst>
 </file>
@@ -10948,7 +10951,7 @@
   <dimension ref="A1:E1702"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1135" workbookViewId="0">
-      <selection activeCell="D1148" sqref="D1148"/>
+      <selection activeCell="D1157" sqref="D1157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -27408,8 +27411,11 @@
       <c r="C1157" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E1157" s="8" t="s">
-        <v>8</v>
+      <c r="D1157" t="s">
+        <v>3493</v>
+      </c>
+      <c r="E1157" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1158" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved a few more problems
</commit_message>
<xml_diff>
--- a/DOCS/Leetcode_FULL.xlsx
+++ b/DOCS/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A234DBD-2CDE-42D8-B8BE-71B66FCB170D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B200E5-57EA-432C-978A-37B161800532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6645" uniqueCount="3525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6645" uniqueCount="3528">
   <si>
     <t>ID</t>
   </si>
@@ -10611,6 +10611,15 @@
   </si>
   <si>
     <t>Recursion</t>
+  </si>
+  <si>
+    <t>Tough to think, important to revise</t>
+  </si>
+  <si>
+    <t>PostOrder Traversal</t>
+  </si>
+  <si>
+    <t>Two Passes</t>
   </si>
 </sst>
 </file>
@@ -11043,8 +11052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1702"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B712" workbookViewId="0">
-      <selection activeCell="D726" sqref="D726"/>
+    <sheetView tabSelected="1" topLeftCell="B123" workbookViewId="0">
+      <selection activeCell="D136" sqref="D136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -13024,8 +13033,11 @@
       <c r="C136" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E136" s="8" t="s">
-        <v>8</v>
+      <c r="D136" t="s">
+        <v>3527</v>
+      </c>
+      <c r="E136" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -24397,8 +24409,11 @@
       <c r="C934" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E934" s="8" t="s">
-        <v>8</v>
+      <c r="D934" t="s">
+        <v>3525</v>
+      </c>
+      <c r="E934" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="935" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -28993,8 +29008,11 @@
       <c r="C1255" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1255" s="8" t="s">
-        <v>8</v>
+      <c r="D1255" t="s">
+        <v>3526</v>
+      </c>
+      <c r="E1255" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1256" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Solved a Few problems
</commit_message>
<xml_diff>
--- a/DOCS/Leetcode_FULL.xlsx
+++ b/DOCS/Leetcode_FULL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\CP-Prac\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E324EB1B-ED53-4B4D-BCBF-96FDD9900D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0AC35A7-C086-46C3-9A5E-02E85C70DF78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6644" uniqueCount="3543">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6644" uniqueCount="3544">
   <si>
     <t>ID</t>
   </si>
@@ -10665,6 +10665,9 @@
   </si>
   <si>
     <t>https://youtu.be/13m9ZCB8gjw</t>
+  </si>
+  <si>
+    <t>DP on Trees, HARD</t>
   </si>
 </sst>
 </file>
@@ -11097,8 +11100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1702"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A207" workbookViewId="0">
-      <selection activeCell="D222" sqref="D222"/>
+    <sheetView tabSelected="1" topLeftCell="A768" workbookViewId="0">
+      <selection activeCell="D781" sqref="D781"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -22312,8 +22315,11 @@
       <c r="C781" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E781" s="8" t="s">
-        <v>8</v>
+      <c r="D781" t="s">
+        <v>3543</v>
+      </c>
+      <c r="E781" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="782" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>